<commit_message>
Exercicios 1.3 e 1.4
</commit_message>
<xml_diff>
--- a/exercicios/1.3/1.3modelagem_fisico.xlsx
+++ b/exercicios/1.3/1.3modelagem_fisico.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C5FF13-E012-41BD-8157-9847EA8EA5E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310E8A45-8FC2-468E-824E-95B95B49AF73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5880" yWindow="-180" windowWidth="12630" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pclinics" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Nome</t>
   </si>
@@ -49,9 +49,6 @@
     <t>CNPJ</t>
   </si>
   <si>
-    <t>Meu Pimpão</t>
-  </si>
-  <si>
     <t>Av. Barão de Limeira, 539</t>
   </si>
   <si>
@@ -106,37 +103,43 @@
     <t>Gato</t>
   </si>
   <si>
-    <t>Poodle</t>
-  </si>
-  <si>
-    <t>Labrador</t>
-  </si>
-  <si>
-    <t>SRD</t>
-  </si>
-  <si>
-    <t>Siamês</t>
-  </si>
-  <si>
-    <t>Junior</t>
-  </si>
-  <si>
-    <t>Loli</t>
-  </si>
-  <si>
-    <t>Sammy</t>
-  </si>
-  <si>
-    <t>Paulo</t>
-  </si>
-  <si>
-    <t>Odirlei</t>
-  </si>
-  <si>
-    <t>Restam 10 dias de vida</t>
-  </si>
-  <si>
     <t>O paciente está ok</t>
+  </si>
+  <si>
+    <t>PETE</t>
+  </si>
+  <si>
+    <t>Rottweiler</t>
+  </si>
+  <si>
+    <t>Pug</t>
+  </si>
+  <si>
+    <t>Bulldog</t>
+  </si>
+  <si>
+    <t>Gato de Manx</t>
+  </si>
+  <si>
+    <t>Thor</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>Nina</t>
+  </si>
+  <si>
+    <t>Mateus Rodrigues</t>
+  </si>
+  <si>
+    <t>Miguel Melo</t>
+  </si>
+  <si>
+    <t>Leonardo Costa</t>
+  </si>
+  <si>
+    <t>Muitas pulgas</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -408,6 +411,10 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,28 +695,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>5</v>
       </c>
@@ -717,14 +725,14 @@
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
       <c r="F1" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -738,42 +746,42 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="15">
+        <v>123456789999</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="15">
-        <v>99999999999999</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H3" s="18">
-        <v>43383</v>
+        <v>40272</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -782,7 +790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -791,10 +799,10 @@
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H4" s="18">
-        <v>42873</v>
+        <v>41858</v>
       </c>
       <c r="I4" s="3">
         <v>4</v>
@@ -803,19 +811,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="26"/>
       <c r="F5" s="3">
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H5" s="18">
-        <v>42537</v>
+        <v>39454</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -824,61 +832,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>22</v>
-      </c>
       <c r="J8" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F9" s="10">
         <v>1</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H9" s="20">
-        <v>43487</v>
+        <v>43895</v>
       </c>
       <c r="I9" s="21">
         <v>1</v>
@@ -887,9 +895,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
@@ -897,10 +905,10 @@
         <v>2</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H10" s="20">
-        <v>43486</v>
+        <v>43996</v>
       </c>
       <c r="I10" s="21">
         <v>2</v>
@@ -909,44 +917,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="10">
         <v>3</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H11" s="20">
-        <v>43487</v>
+        <v>44218</v>
       </c>
       <c r="I11" s="21">
         <v>2</v>
       </c>
       <c r="J11" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>2</v>
       </c>
@@ -957,17 +965,17 @@
         <v>1</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="22"/>
       <c r="I13" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="23"/>
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>3</v>
       </c>
@@ -978,25 +986,25 @@
         <v>1</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J14" s="17" t="s">
         <v>0</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L14" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>4</v>
       </c>
@@ -1010,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I15" s="19">
         <v>1</v>
@@ -1019,18 +1027,18 @@
         <v>2</v>
       </c>
       <c r="K15" s="19">
-        <v>432551</v>
+        <v>123456</v>
       </c>
       <c r="L15" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F16" s="12">
         <v>2</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I16" s="19">
         <v>2</v>
@@ -1039,10 +1047,18 @@
         <v>3</v>
       </c>
       <c r="K16" s="19">
-        <v>653655</v>
+        <v>654321</v>
       </c>
       <c r="L16" s="19">
         <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="29">
+        <v>3</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>